<commit_message>
Subimos el proyecto final
</commit_message>
<xml_diff>
--- a/PR02/Enunciado/DAW2 - Projectes - Enunciat PR02.xlsx
+++ b/PR02/Enunciado/DAW2 - Projectes - Enunciat PR02.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DAW2\Proyectos\PR02\Enunciado\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DAW36929\Projecte02\Proyecto3-master\PR02\Enunciado\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -270,7 +270,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -421,22 +421,22 @@
     <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,7 +471,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="image2.jpg" title="Imatge"/>
+        <xdr:cNvPr id="2" name="image2.jpg" title="Imatge">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -508,7 +514,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="image1.jpg" title="Imatge"/>
+        <xdr:cNvPr id="3" name="image1.jpg" title="Imatge">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -545,7 +557,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="image3.jpg" title="Imatge"/>
+        <xdr:cNvPr id="4" name="image3.jpg" title="Imatge">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -582,7 +600,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="image4.jpg" title="Imatge"/>
+        <xdr:cNvPr id="5" name="image4.jpg" title="Imatge">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -619,7 +643,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="image5.jpg" title="Imatge"/>
+        <xdr:cNvPr id="6" name="image5.jpg" title="Imatge">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -656,7 +686,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="image6.jpg" title="Imatge"/>
+        <xdr:cNvPr id="7" name="image6.jpg" title="Imatge">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -693,7 +729,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="image7.jpg" title="Imatge"/>
+        <xdr:cNvPr id="8" name="image7.jpg" title="Imatge">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -730,7 +772,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="image8.jpg" title="Imatge"/>
+        <xdr:cNvPr id="9" name="image8.jpg" title="Imatge">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1020,14 +1068,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:I12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="6" customWidth="1"/>
+    <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
     <col min="10" max="15" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1043,7 +1091,7 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="9"/>
@@ -1077,65 +1125,65 @@
       <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="17" t="s">
         <v>9</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:15" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="9"/>
@@ -1164,17 +1212,17 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
       <c r="K10" s="7" t="s">
         <v>18</v>
       </c>
@@ -1189,15 +1237,15 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
       <c r="K11" s="7" t="s">
         <v>22</v>
       </c>
@@ -1211,15 +1259,15 @@
       <c r="O11" s="7"/>
     </row>
     <row r="12" spans="1:15" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
@@ -1234,7 +1282,7 @@
       <c r="O13" s="7"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="9"/>
@@ -1264,17 +1312,17 @@
       <c r="O14" s="7"/>
     </row>
     <row r="15" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
       <c r="K15" s="7" t="s">
         <v>31</v>
       </c>
@@ -1290,15 +1338,15 @@
       <c r="O15" s="7"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
       <c r="K16" s="7" t="s">
         <v>35</v>
       </c>
@@ -1314,15 +1362,15 @@
       <c r="O16" s="7"/>
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
@@ -1336,7 +1384,7 @@
       <c r="O18" s="7"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="13" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="9"/>
@@ -1353,43 +1401,43 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
     </row>
     <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="15" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="9"/>
@@ -1406,43 +1454,43 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B29" s="9"/>
@@ -1459,39 +1507,39 @@
       </c>
     </row>
     <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2463,6 +2511,11 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A4:I7"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A15:I17"/>
     <mergeCell ref="A29:G29"/>
     <mergeCell ref="A30:I32"/>
     <mergeCell ref="A20:I22"/>
@@ -2471,11 +2524,6 @@
     <mergeCell ref="A10:I12"/>
     <mergeCell ref="A25:I27"/>
     <mergeCell ref="A24:G24"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="A4:I7"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A15:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>